<commit_message>
se agregan comentarios enge y se calcula brecha vs eeuu
</commit_message>
<xml_diff>
--- a/results/enge/enge_results.xlsx
+++ b/results/enge/enge_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W253"/>
+  <dimension ref="A1:X253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +544,11 @@
           <t>productividad_ipi_index_1</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -617,6 +622,11 @@
       <c r="W2" t="n">
         <v>0.9655375273883546</v>
       </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -690,6 +700,11 @@
       <c r="W3" t="n">
         <v>0.6731992824876608</v>
       </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -763,6 +778,11 @@
       <c r="W4" t="n">
         <v>0.5911606616726508</v>
       </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -836,6 +856,11 @@
       <c r="W5" t="n">
         <v>0.5403726227743313</v>
       </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -909,6 +934,11 @@
       <c r="W6" t="n">
         <v>0.9306764790622576</v>
       </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -982,6 +1012,11 @@
       <c r="W7" t="n">
         <v>0.7541752382287841</v>
       </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1055,6 +1090,11 @@
       <c r="W8" t="n">
         <v>0.7218964618804438</v>
       </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1128,6 +1168,11 @@
       <c r="W9" t="n">
         <v>0.7244387001599271</v>
       </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1201,6 +1246,11 @@
       <c r="W10" t="n">
         <v>0.7988607932690958</v>
       </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1274,6 +1324,11 @@
       <c r="W11" t="n">
         <v>1.078368147508145</v>
       </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1347,6 +1402,11 @@
       <c r="W12" t="n">
         <v>0.8096637639524709</v>
       </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1420,6 +1480,11 @@
       <c r="W13" t="n">
         <v>0.7939084002339221</v>
       </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1493,6 +1558,11 @@
       <c r="W14" t="n">
         <v>0.7101334971865104</v>
       </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1566,6 +1636,11 @@
       <c r="W15" t="n">
         <v>1.014771538295683</v>
       </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1639,6 +1714,11 @@
       <c r="W16" t="n">
         <v>0.7684435587207532</v>
       </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1712,6 +1792,11 @@
       <c r="W17" t="n">
         <v>0.8784292909638097</v>
       </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1785,6 +1870,11 @@
       <c r="W18" t="n">
         <v>0.8613973724449109</v>
       </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1858,6 +1948,11 @@
       <c r="W19" t="n">
         <v>0.9167468223943485</v>
       </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1931,6 +2026,11 @@
       <c r="W20" t="n">
         <v>1.053034401221038</v>
       </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2004,6 +2104,11 @@
       <c r="W21" t="n">
         <v>0.7848728463237061</v>
       </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2077,6 +2182,11 @@
       <c r="W22" t="n">
         <v>0.8774549125206896</v>
       </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2150,6 +2260,11 @@
       <c r="W23" t="n">
         <v>0.9345397471694883</v>
       </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2223,6 +2338,11 @@
       <c r="W24" t="n">
         <v>0.634100720474478</v>
       </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2296,6 +2416,11 @@
       <c r="W25" t="n">
         <v>0.8255390804799508</v>
       </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2369,6 +2494,11 @@
       <c r="W26" t="n">
         <v>0.9182595789787379</v>
       </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2442,6 +2572,11 @@
       <c r="W27" t="n">
         <v>0.8776842260573566</v>
       </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2515,6 +2650,11 @@
       <c r="W28" t="n">
         <v>0.860886066032405</v>
       </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2588,6 +2728,11 @@
       <c r="W29" t="n">
         <v>1.052401414151967</v>
       </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2661,6 +2806,11 @@
       <c r="W30" t="n">
         <v>0.8404838039910085</v>
       </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2734,6 +2884,11 @@
       <c r="W31" t="n">
         <v>0.9537781760251646</v>
       </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2807,6 +2962,11 @@
       <c r="W32" t="n">
         <v>0.9141849171767609</v>
       </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2880,6 +3040,11 @@
       <c r="W33" t="n">
         <v>0.92653357422214</v>
       </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2953,6 +3118,11 @@
       <c r="W34" t="n">
         <v>1.011381710870384</v>
       </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3026,6 +3196,11 @@
       <c r="W35" t="n">
         <v>0.9538669945303954</v>
       </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3099,6 +3274,11 @@
       <c r="W36" t="n">
         <v>0.9457378903202371</v>
       </c>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3172,6 +3352,11 @@
       <c r="W37" t="n">
         <v>0.9306417416789843</v>
       </c>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3245,6 +3430,11 @@
       <c r="W38" t="n">
         <v>1</v>
       </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3318,6 +3508,11 @@
       <c r="W39" t="n">
         <v>1</v>
       </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3391,6 +3586,11 @@
       <c r="W40" t="n">
         <v>1</v>
       </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3464,6 +3664,11 @@
       <c r="W41" t="n">
         <v>1</v>
       </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3537,6 +3742,11 @@
       <c r="W42" t="n">
         <v>1</v>
       </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3610,6 +3820,11 @@
       <c r="W43" t="n">
         <v>1</v>
       </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -3683,6 +3898,11 @@
       <c r="W44" t="n">
         <v>1</v>
       </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -3756,6 +3976,11 @@
       <c r="W45" t="n">
         <v>1</v>
       </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -3829,6 +4054,11 @@
       <c r="W46" t="n">
         <v>1</v>
       </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -3902,6 +4132,11 @@
       <c r="W47" t="n">
         <v>1.050420006487289</v>
       </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -3975,6 +4210,11 @@
       <c r="W48" t="n">
         <v>1.026311496182025</v>
       </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -4048,6 +4288,11 @@
       <c r="W49" t="n">
         <v>1.220514414577789</v>
       </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -4121,6 +4366,11 @@
       <c r="W50" t="n">
         <v>1.160556178404059</v>
       </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -4194,6 +4444,11 @@
       <c r="W51" t="n">
         <v>1.063795060754388</v>
       </c>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -4267,6 +4522,11 @@
       <c r="W52" t="n">
         <v>0.8124811609440555</v>
       </c>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -4340,6 +4600,11 @@
       <c r="W53" t="n">
         <v>1.031684161244126</v>
       </c>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -4413,6 +4678,11 @@
       <c r="W54" t="n">
         <v>1.005167959014127</v>
       </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -4486,6 +4756,11 @@
       <c r="W55" t="n">
         <v>1.043714802794835</v>
       </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -4559,6 +4834,11 @@
       <c r="W56" t="n">
         <v>1.082198391783598</v>
       </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -4632,6 +4912,11 @@
       <c r="W57" t="n">
         <v>1.014382248630605</v>
       </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -4705,6 +4990,11 @@
       <c r="W58" t="n">
         <v>1.253738428916553</v>
       </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -4778,6 +5068,11 @@
       <c r="W59" t="n">
         <v>1.230110493462278</v>
       </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -4851,6 +5146,11 @@
       <c r="W60" t="n">
         <v>0.7296488740491788</v>
       </c>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -4924,6 +5224,11 @@
       <c r="W61" t="n">
         <v>1.255519191657036</v>
       </c>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -4997,6 +5302,11 @@
       <c r="W62" t="n">
         <v>1.01552230130252</v>
       </c>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -5070,6 +5380,11 @@
       <c r="W63" t="n">
         <v>1.021274002929934</v>
       </c>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -5143,6 +5458,11 @@
       <c r="W64" t="n">
         <v>1.00864581167729</v>
       </c>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -5216,6 +5536,11 @@
       <c r="W65" t="n">
         <v>1.127615387974315</v>
       </c>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -5289,6 +5614,11 @@
       <c r="W66" t="n">
         <v>1.064128047677501</v>
       </c>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -5362,6 +5692,11 @@
       <c r="W67" t="n">
         <v>1.095819390336142</v>
       </c>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -5435,6 +5770,11 @@
       <c r="W68" t="n">
         <v>1.237291531096817</v>
       </c>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -5508,6 +5848,11 @@
       <c r="W69" t="n">
         <v>0.974310682436092</v>
       </c>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -5581,6 +5926,11 @@
       <c r="W70" t="n">
         <v>1.904977616332479</v>
       </c>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -5654,6 +6004,11 @@
       <c r="W71" t="n">
         <v>0.9871603807878383</v>
       </c>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -5727,6 +6082,11 @@
       <c r="W72" t="n">
         <v>1.095343774399946</v>
       </c>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -5800,6 +6160,11 @@
       <c r="W73" t="n">
         <v>1.097636094753893</v>
       </c>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -5873,6 +6238,11 @@
       <c r="W74" t="n">
         <v>1.075225920511548</v>
       </c>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -5946,6 +6316,11 @@
       <c r="W75" t="n">
         <v>1.124106656160287</v>
       </c>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -6019,6 +6394,11 @@
       <c r="W76" t="n">
         <v>1.10894911170732</v>
       </c>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -6092,6 +6472,11 @@
       <c r="W77" t="n">
         <v>1.233433510010398</v>
       </c>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -6165,6 +6550,11 @@
       <c r="W78" t="n">
         <v>0.6193886145464567</v>
       </c>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -6238,6 +6628,11 @@
       <c r="W79" t="n">
         <v>1.5328209294666</v>
       </c>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -6311,6 +6706,11 @@
       <c r="W80" t="n">
         <v>0.9654351318750515</v>
       </c>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -6384,6 +6784,11 @@
       <c r="W81" t="n">
         <v>1.055058494816057</v>
       </c>
+      <c r="X81" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -6457,6 +6862,11 @@
       <c r="W82" t="n">
         <v>1.089410039665801</v>
       </c>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -6530,6 +6940,11 @@
       <c r="W83" t="n">
         <v>1.387218373968457</v>
       </c>
+      <c r="X83" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -6603,6 +7018,11 @@
       <c r="W84" t="n">
         <v>1.13399164065861</v>
       </c>
+      <c r="X84" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -6676,6 +7096,11 @@
       <c r="W85" t="n">
         <v>0.7705188231540495</v>
       </c>
+      <c r="X85" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -6749,6 +7174,11 @@
       <c r="W86" t="n">
         <v>0.7849609808059061</v>
       </c>
+      <c r="X86" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -6822,6 +7252,11 @@
       <c r="W87" t="n">
         <v>1.023279799175007</v>
       </c>
+      <c r="X87" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -6895,6 +7330,11 @@
       <c r="W88" t="n">
         <v>2.07916378034938</v>
       </c>
+      <c r="X88" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -6968,6 +7408,11 @@
       <c r="W89" t="n">
         <v>0.8279455069117995</v>
       </c>
+      <c r="X89" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -7041,6 +7486,11 @@
       <c r="W90" t="n">
         <v>1.190320567084726</v>
       </c>
+      <c r="X90" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -7114,6 +7564,11 @@
       <c r="W91" t="n">
         <v>1.338052881439008</v>
       </c>
+      <c r="X91" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -7187,6 +7642,11 @@
       <c r="W92" t="n">
         <v>1.464019743551098</v>
       </c>
+      <c r="X92" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -7260,6 +7720,11 @@
       <c r="W93" t="n">
         <v>1.328976902859728</v>
       </c>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -7333,6 +7798,11 @@
       <c r="W94" t="n">
         <v>0.7856606717675199</v>
       </c>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -7406,6 +7876,11 @@
       <c r="W95" t="n">
         <v>0.7985576818800064</v>
       </c>
+      <c r="X95" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -7479,6 +7954,11 @@
       <c r="W96" t="n">
         <v>0.9424922783362482</v>
       </c>
+      <c r="X96" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -7552,6 +8032,11 @@
       <c r="W97" t="n">
         <v>1.673700861911638</v>
       </c>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -7625,6 +8110,11 @@
       <c r="W98" t="n">
         <v>0.8319922705486268</v>
       </c>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -7698,6 +8188,11 @@
       <c r="W99" t="n">
         <v>1.232092421892111</v>
       </c>
+      <c r="X99" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -7771,6 +8266,11 @@
       <c r="W100" t="n">
         <v>1.404861621330227</v>
       </c>
+      <c r="X100" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -7844,6 +8344,11 @@
       <c r="W101" t="n">
         <v>1.491350345340075</v>
       </c>
+      <c r="X101" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -7917,6 +8422,11 @@
       <c r="W102" t="n">
         <v>1.48520725279597</v>
       </c>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -7990,6 +8500,11 @@
       <c r="W103" t="n">
         <v>0.7958871658995581</v>
       </c>
+      <c r="X103" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -8063,6 +8578,11 @@
       <c r="W104" t="n">
         <v>0.8322876270227909</v>
       </c>
+      <c r="X104" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -8136,6 +8656,11 @@
       <c r="W105" t="n">
         <v>1.21923263170246</v>
       </c>
+      <c r="X105" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -8209,6 +8734,11 @@
       <c r="W106" t="n">
         <v>1.6835107179942</v>
       </c>
+      <c r="X106" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -8282,6 +8812,11 @@
       <c r="W107" t="n">
         <v>0.8893217887802174</v>
       </c>
+      <c r="X107" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -8355,6 +8890,11 @@
       <c r="W108" t="n">
         <v>1.30568124751747</v>
       </c>
+      <c r="X108" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -8428,6 +8968,11 @@
       <c r="W109" t="n">
         <v>1.539949830059086</v>
       </c>
+      <c r="X109" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -8501,6 +9046,11 @@
       <c r="W110" t="n">
         <v>1.54352777085219</v>
       </c>
+      <c r="X110" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -8574,6 +9124,11 @@
       <c r="W111" t="n">
         <v>1.453042463104012</v>
       </c>
+      <c r="X111" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -8647,6 +9202,11 @@
       <c r="W112" t="n">
         <v>0.9048596361641909</v>
       </c>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -8720,6 +9280,11 @@
       <c r="W113" t="n">
         <v>0.9187766876929342</v>
       </c>
+      <c r="X113" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -8793,6 +9358,11 @@
       <c r="W114" t="n">
         <v>1.26285122020636</v>
       </c>
+      <c r="X114" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -8866,6 +9436,11 @@
       <c r="W115" t="n">
         <v>1.474803127857875</v>
       </c>
+      <c r="X115" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -8939,6 +9514,11 @@
       <c r="W116" t="n">
         <v>0.9341430541362958</v>
       </c>
+      <c r="X116" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -9012,6 +9592,11 @@
       <c r="W117" t="n">
         <v>1.35696054762719</v>
       </c>
+      <c r="X117" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -9085,6 +9670,11 @@
       <c r="W118" t="n">
         <v>1.546552338021762</v>
       </c>
+      <c r="X118" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -9158,6 +9748,11 @@
       <c r="W119" t="n">
         <v>1.564391486496064</v>
       </c>
+      <c r="X119" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -9231,6 +9826,11 @@
       <c r="W120" t="n">
         <v>1.461639811733402</v>
       </c>
+      <c r="X120" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -9304,6 +9904,11 @@
       <c r="W121" t="n">
         <v>0.982949508679922</v>
       </c>
+      <c r="X121" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -9377,6 +9982,11 @@
       <c r="W122" t="n">
         <v>0.9783204449531475</v>
       </c>
+      <c r="X122" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -9450,6 +10060,11 @@
       <c r="W123" t="n">
         <v>1.3319189477687</v>
       </c>
+      <c r="X123" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -9523,6 +10138,11 @@
       <c r="W124" t="n">
         <v>1.59424955356755</v>
       </c>
+      <c r="X124" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -9596,6 +10216,11 @@
       <c r="W125" t="n">
         <v>1.005418329190879</v>
       </c>
+      <c r="X125" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -9669,6 +10294,11 @@
       <c r="W126" t="n">
         <v>1.409009831082886</v>
       </c>
+      <c r="X126" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -9742,6 +10372,11 @@
       <c r="W127" t="n">
         <v>1.569236191629599</v>
       </c>
+      <c r="X127" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -9815,6 +10450,11 @@
       <c r="W128" t="n">
         <v>1.918053866271535</v>
       </c>
+      <c r="X128" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -9888,6 +10528,11 @@
       <c r="W129" t="n">
         <v>1.483759714284771</v>
       </c>
+      <c r="X129" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -9961,6 +10606,11 @@
       <c r="W130" t="n">
         <v>1.082046570231265</v>
       </c>
+      <c r="X130" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -10034,6 +10684,11 @@
       <c r="W131" t="n">
         <v>1.010732489424514</v>
       </c>
+      <c r="X131" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -10107,6 +10762,11 @@
       <c r="W132" t="n">
         <v>1.446984433684948</v>
       </c>
+      <c r="X132" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -10180,6 +10840,11 @@
       <c r="W133" t="n">
         <v>1.261296472332019</v>
       </c>
+      <c r="X133" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -10253,6 +10918,11 @@
       <c r="W134" t="n">
         <v>1.040747341883922</v>
       </c>
+      <c r="X134" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -10326,6 +10996,11 @@
       <c r="W135" t="n">
         <v>1.418363373133066</v>
       </c>
+      <c r="X135" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -10399,6 +11074,11 @@
       <c r="W136" t="n">
         <v>1.684543800404557</v>
       </c>
+      <c r="X136" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -10472,6 +11152,11 @@
       <c r="W137" t="n">
         <v>1.889237365881537</v>
       </c>
+      <c r="X137" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -10545,6 +11230,11 @@
       <c r="W138" t="n">
         <v>1.61597505724605</v>
       </c>
+      <c r="X138" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -10618,6 +11308,11 @@
       <c r="W139" t="n">
         <v>1.062061705269974</v>
       </c>
+      <c r="X139" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -10691,6 +11386,11 @@
       <c r="W140" t="n">
         <v>0.8888609649453856</v>
       </c>
+      <c r="X140" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -10764,6 +11464,11 @@
       <c r="W141" t="n">
         <v>1.259022966545505</v>
       </c>
+      <c r="X141" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -10837,6 +11542,11 @@
       <c r="W142" t="n">
         <v>1.012705126069556</v>
       </c>
+      <c r="X142" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -10910,6 +11620,11 @@
       <c r="W143" t="n">
         <v>0.9924237083443946</v>
       </c>
+      <c r="X143" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -10983,6 +11698,11 @@
       <c r="W144" t="n">
         <v>1.335201455961898</v>
       </c>
+      <c r="X144" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -11056,6 +11776,11 @@
       <c r="W145" t="n">
         <v>1.691540514014277</v>
       </c>
+      <c r="X145" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -11129,6 +11854,11 @@
       <c r="W146" t="n">
         <v>1.9034095054665</v>
       </c>
+      <c r="X146" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -11202,6 +11932,11 @@
       <c r="W147" t="n">
         <v>1.368200951273467</v>
       </c>
+      <c r="X147" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -11275,6 +12010,11 @@
       <c r="W148" t="n">
         <v>1.154420968654192</v>
       </c>
+      <c r="X148" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -11348,6 +12088,11 @@
       <c r="W149" t="n">
         <v>0.8591192943006982</v>
       </c>
+      <c r="X149" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -11421,6 +12166,11 @@
       <c r="W150" t="n">
         <v>1.056545289247847</v>
       </c>
+      <c r="X150" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -11494,6 +12244,11 @@
       <c r="W151" t="n">
         <v>1.091375128846194</v>
       </c>
+      <c r="X151" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -11567,6 +12322,11 @@
       <c r="W152" t="n">
         <v>0.9918571540428023</v>
       </c>
+      <c r="X152" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -11640,6 +12400,11 @@
       <c r="W153" t="n">
         <v>1.286011129670423</v>
       </c>
+      <c r="X153" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -11713,6 +12478,11 @@
       <c r="W154" t="n">
         <v>1.542332923687951</v>
       </c>
+      <c r="X154" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -11786,6 +12556,11 @@
       <c r="W155" t="n">
         <v>1.982335373471905</v>
       </c>
+      <c r="X155" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -11859,6 +12634,11 @@
       <c r="W156" t="n">
         <v>1.402634340663601</v>
       </c>
+      <c r="X156" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -11932,6 +12712,11 @@
       <c r="W157" t="n">
         <v>1.452507578058224</v>
       </c>
+      <c r="X157" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -12005,6 +12790,11 @@
       <c r="W158" t="n">
         <v>0.7174541925227401</v>
       </c>
+      <c r="X158" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -12078,6 +12868,11 @@
       <c r="W159" t="n">
         <v>1.277501261727035</v>
       </c>
+      <c r="X159" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -12151,6 +12946,11 @@
       <c r="W160" t="n">
         <v>1.153489609035821</v>
       </c>
+      <c r="X160" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -12224,6 +13024,11 @@
       <c r="W161" t="n">
         <v>1.033244610476908</v>
       </c>
+      <c r="X161" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -12297,6 +13102,11 @@
       <c r="W162" t="n">
         <v>1.330002046956783</v>
       </c>
+      <c r="X162" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -12370,6 +13180,11 @@
       <c r="W163" t="n">
         <v>1.615982529519189</v>
       </c>
+      <c r="X163" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -12443,6 +13258,11 @@
       <c r="W164" t="n">
         <v>2.12940362473096</v>
       </c>
+      <c r="X164" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -12516,6 +13336,11 @@
       <c r="W165" t="n">
         <v>1.481532968611714</v>
       </c>
+      <c r="X165" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -12589,6 +13414,11 @@
       <c r="W166" t="n">
         <v>1.404303180961416</v>
       </c>
+      <c r="X166" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -12662,6 +13492,11 @@
       <c r="W167" t="n">
         <v>0.7277757631668669</v>
       </c>
+      <c r="X167" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -12735,6 +13570,11 @@
       <c r="W168" t="n">
         <v>1.238162626455064</v>
       </c>
+      <c r="X168" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -12808,6 +13648,11 @@
       <c r="W169" t="n">
         <v>1.002033666848277</v>
       </c>
+      <c r="X169" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -12881,6 +13726,11 @@
       <c r="W170" t="n">
         <v>1.038098191937751</v>
       </c>
+      <c r="X170" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -12954,6 +13804,11 @@
       <c r="W171" t="n">
         <v>1.313966037778414</v>
       </c>
+      <c r="X171" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -13027,6 +13882,11 @@
       <c r="W172" t="n">
         <v>1.647347453155421</v>
       </c>
+      <c r="X172" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -13100,6 +13960,11 @@
       <c r="W173" t="n">
         <v>2.047761875555398</v>
       </c>
+      <c r="X173" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -13173,6 +14038,11 @@
       <c r="W174" t="n">
         <v>1.400021245361283</v>
       </c>
+      <c r="X174" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -13246,6 +14116,11 @@
       <c r="W175" t="n">
         <v>1.256814820432401</v>
       </c>
+      <c r="X175" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -13319,6 +14194,11 @@
       <c r="W176" t="n">
         <v>0.6629294982278614</v>
       </c>
+      <c r="X176" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -13392,6 +14272,11 @@
       <c r="W177" t="n">
         <v>1.338766912605683</v>
       </c>
+      <c r="X177" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -13465,6 +14350,11 @@
       <c r="W178" t="n">
         <v>0.8938949334411623</v>
       </c>
+      <c r="X178" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -13538,6 +14428,11 @@
       <c r="W179" t="n">
         <v>1.028763983781385</v>
       </c>
+      <c r="X179" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -13611,6 +14506,11 @@
       <c r="W180" t="n">
         <v>1.293970578802475</v>
       </c>
+      <c r="X180" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -13684,6 +14584,11 @@
       <c r="W181" t="n">
         <v>1.625592369551838</v>
       </c>
+      <c r="X181" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -13757,6 +14662,11 @@
       <c r="W182" t="n">
         <v>2.020203212002306</v>
       </c>
+      <c r="X182" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -13830,6 +14740,11 @@
       <c r="W183" t="n">
         <v>1.257784961654216</v>
       </c>
+      <c r="X183" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -13903,6 +14818,11 @@
       <c r="W184" t="n">
         <v>1.18598565002453</v>
       </c>
+      <c r="X184" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -13976,6 +14896,11 @@
       <c r="W185" t="n">
         <v>0.680711298572792</v>
       </c>
+      <c r="X185" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -14049,6 +14974,11 @@
       <c r="W186" t="n">
         <v>1.473801078905665</v>
       </c>
+      <c r="X186" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -14122,6 +15052,11 @@
       <c r="W187" t="n">
         <v>0.7789845685990204</v>
       </c>
+      <c r="X187" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -14195,6 +15130,11 @@
       <c r="W188" t="n">
         <v>1.04256773762082</v>
       </c>
+      <c r="X188" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -14268,6 +15208,11 @@
       <c r="W189" t="n">
         <v>1.271384651940365</v>
       </c>
+      <c r="X189" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -14341,6 +15286,11 @@
       <c r="W190" t="n">
         <v>1.607676472214792</v>
       </c>
+      <c r="X190" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -14414,6 +15364,11 @@
       <c r="W191" t="n">
         <v>1.999776707210901</v>
       </c>
+      <c r="X191" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -14487,6 +15442,11 @@
       <c r="W192" t="n">
         <v>1.280878656891056</v>
       </c>
+      <c r="X192" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -14560,6 +15520,11 @@
       <c r="W193" t="n">
         <v>1.095419306952935</v>
       </c>
+      <c r="X193" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -14633,6 +15598,11 @@
       <c r="W194" t="n">
         <v>0.6259179137554093</v>
       </c>
+      <c r="X194" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -14706,6 +15676,11 @@
       <c r="W195" t="n">
         <v>1.128535330100045</v>
       </c>
+      <c r="X195" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -14779,6 +15754,11 @@
       <c r="W196" t="n">
         <v>0.701838255915197</v>
       </c>
+      <c r="X196" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -14852,6 +15832,11 @@
       <c r="W197" t="n">
         <v>0.9735425436345349</v>
       </c>
+      <c r="X197" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -14925,6 +15910,11 @@
       <c r="W198" t="n">
         <v>1.228014418541406</v>
       </c>
+      <c r="X198" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -14998,6 +15988,11 @@
       <c r="W199" t="n">
         <v>1.583327508925176</v>
       </c>
+      <c r="X199" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -15071,6 +16066,11 @@
       <c r="W200" t="n">
         <v>1.971748073326323</v>
       </c>
+      <c r="X200" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -15144,6 +16144,11 @@
       <c r="W201" t="n">
         <v>1.261039669100112</v>
       </c>
+      <c r="X201" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -15217,6 +16222,11 @@
       <c r="W202" t="n">
         <v>1.153974841070407</v>
       </c>
+      <c r="X202" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -15290,6 +16300,11 @@
       <c r="W203" t="n">
         <v>0.6443245224476318</v>
       </c>
+      <c r="X203" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -15363,6 +16378,11 @@
       <c r="W204" t="n">
         <v>1.503902457790673</v>
       </c>
+      <c r="X204" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -15436,6 +16456,11 @@
       <c r="W205" t="n">
         <v>0.5245267334707208</v>
       </c>
+      <c r="X205" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -15509,6 +16534,11 @@
       <c r="W206" t="n">
         <v>1.016342318043133</v>
       </c>
+      <c r="X206" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -15582,6 +16612,11 @@
       <c r="W207" t="n">
         <v>1.204558112716535</v>
       </c>
+      <c r="X207" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -15655,6 +16690,11 @@
       <c r="W208" t="n">
         <v>1.605523046512494</v>
       </c>
+      <c r="X208" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -15728,6 +16768,11 @@
       <c r="W209" t="n">
         <v>1.83317694780462</v>
       </c>
+      <c r="X209" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -15801,6 +16846,11 @@
       <c r="W210" t="n">
         <v>1.271466184725924</v>
       </c>
+      <c r="X210" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -15874,6 +16924,11 @@
       <c r="W211" t="n">
         <v>1.27890563600768</v>
       </c>
+      <c r="X211" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -15947,6 +17002,11 @@
       <c r="W212" t="n">
         <v>0.8170498368068068</v>
       </c>
+      <c r="X212" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -16020,6 +17080,11 @@
       <c r="W213" t="n">
         <v>1.520490756516</v>
       </c>
+      <c r="X213" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -16093,6 +17158,11 @@
       <c r="W214" t="n">
         <v>0.5897192865178299</v>
       </c>
+      <c r="X214" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -16166,6 +17236,11 @@
       <c r="W215" t="n">
         <v>0.871257308731925</v>
       </c>
+      <c r="X215" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -16239,6 +17314,11 @@
       <c r="W216" t="n">
         <v>1.171540685253981</v>
       </c>
+      <c r="X216" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -16312,6 +17392,11 @@
       <c r="W217" t="n">
         <v>1.562292589337589</v>
       </c>
+      <c r="X217" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -16385,6 +17470,11 @@
       <c r="W218" t="n">
         <v>1.964434689653546</v>
       </c>
+      <c r="X218" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -16458,6 +17548,11 @@
       <c r="W219" t="n">
         <v>1.302830110471927</v>
       </c>
+      <c r="X219" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -16531,6 +17626,11 @@
       <c r="W220" t="n">
         <v>1.020066261964222</v>
       </c>
+      <c r="X220" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -16604,6 +17704,11 @@
       <c r="W221" t="n">
         <v>0.8790503144275732</v>
       </c>
+      <c r="X221" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -16677,6 +17782,11 @@
       <c r="W222" t="n">
         <v>1.588439721668349</v>
       </c>
+      <c r="X222" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -16750,6 +17860,11 @@
       <c r="W223" t="n">
         <v>0.8053342768609437</v>
       </c>
+      <c r="X223" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -16823,6 +17938,11 @@
       <c r="W224" t="n">
         <v>0.8291719072665895</v>
       </c>
+      <c r="X224" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -16896,6 +18016,11 @@
       <c r="W225" t="n">
         <v>1.231345752191737</v>
       </c>
+      <c r="X225" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -16969,6 +18094,11 @@
       <c r="W226" t="n">
         <v>1.663975013867216</v>
       </c>
+      <c r="X226" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -17042,6 +18172,11 @@
       <c r="W227" t="n">
         <v>2.002519235046935</v>
       </c>
+      <c r="X227" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -17115,6 +18250,11 @@
       <c r="W228" t="n">
         <v>1.322641776236642</v>
       </c>
+      <c r="X228" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -17188,6 +18328,11 @@
       <c r="W229" t="n">
         <v>1.000058304434054</v>
       </c>
+      <c r="X229" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -17261,6 +18406,11 @@
       <c r="W230" t="n">
         <v>0.8253003842453235</v>
       </c>
+      <c r="X230" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -17334,6 +18484,11 @@
       <c r="W231" t="n">
         <v>1.475857609379086</v>
       </c>
+      <c r="X231" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -17407,6 +18562,11 @@
       <c r="W232" t="n">
         <v>0.7410701716624302</v>
       </c>
+      <c r="X232" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -17480,6 +18640,11 @@
       <c r="W233" t="n">
         <v>0.7977078786776125</v>
       </c>
+      <c r="X233" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -17553,6 +18718,11 @@
       <c r="W234" t="n">
         <v>1.208622469854537</v>
       </c>
+      <c r="X234" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -17626,6 +18796,11 @@
       <c r="W235" t="n">
         <v>1.690650460046172</v>
       </c>
+      <c r="X235" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -17699,6 +18874,11 @@
       <c r="W236" t="n">
         <v>1.843293001828729</v>
       </c>
+      <c r="X236" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -17772,6 +18952,11 @@
       <c r="W237" t="n">
         <v>1.074016544985437</v>
       </c>
+      <c r="X237" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -17845,6 +19030,11 @@
       <c r="W238" t="n">
         <v>0.9546865390859003</v>
       </c>
+      <c r="X238" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -17918,6 +19108,11 @@
       <c r="W239" t="n">
         <v>0.7713819713825384</v>
       </c>
+      <c r="X239" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -17991,6 +19186,11 @@
       <c r="W240" t="n">
         <v>1.230764811695587</v>
       </c>
+      <c r="X240" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -18064,6 +19264,11 @@
       <c r="W241" t="n">
         <v>0.5448373517075934</v>
       </c>
+      <c r="X241" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -18137,6 +19342,11 @@
       <c r="W242" t="n">
         <v>0.740247200548581</v>
       </c>
+      <c r="X242" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -18210,6 +19420,11 @@
       <c r="W243" t="n">
         <v>1.052128415987211</v>
       </c>
+      <c r="X243" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -18283,6 +19498,11 @@
       <c r="W244" t="n">
         <v>1.461769233885915</v>
       </c>
+      <c r="X244" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -18356,6 +19576,11 @@
       <c r="W245" t="n">
         <v>1.821892413588448</v>
       </c>
+      <c r="X245" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -18429,6 +19654,11 @@
       <c r="W246" t="n">
         <v>1.012338410252521</v>
       </c>
+      <c r="X246" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -18502,6 +19732,11 @@
       <c r="W247" t="n">
         <v>0.7713892554142985</v>
       </c>
+      <c r="X247" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -18575,6 +19810,11 @@
       <c r="W248" t="n">
         <v>0.6345330493942476</v>
       </c>
+      <c r="X248" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -18648,6 +19888,11 @@
       <c r="W249" t="n">
         <v>1.294474463857231</v>
       </c>
+      <c r="X249" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -18721,6 +19966,11 @@
       <c r="W250" t="n">
         <v>0.6070513764618353</v>
       </c>
+      <c r="X250" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -18794,6 +20044,11 @@
       <c r="W251" t="n">
         <v>0.7066852654704837</v>
       </c>
+      <c r="X251" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -18867,6 +20122,11 @@
       <c r="W252" t="n">
         <v>1.041035771270268</v>
       </c>
+      <c r="X252" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -18939,6 +20199,11 @@
       </c>
       <c r="W253" t="n">
         <v>1.440841859756294</v>
+      </c>
+      <c r="X253" t="inlineStr">
+        <is>
+          <t>Valor Agregado Bruto (vab) en pesos corrientes y luego ajustado o convertido por distintas variables (IPC, IPI, TCP, TCC). Empleo en puestos de trabajo asalariados (emp). La productividad del trabajo se presenta tanto en índice como en nivel.</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>